<commit_message>
updated timeline_data.yml and test_timeline.xlsx
</commit_message>
<xml_diff>
--- a/_data/test_timeline.xlsx
+++ b/_data/test_timeline.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="93">
   <si>
     <t>title</t>
   </si>
@@ -277,6 +277,15 @@
   </si>
   <si>
     <t>https://lh3.googleusercontent.com/9Bmkbckei5H4aSRe7OGZKdpziaS4UlhcZdts7StG03oI52pCl7jbu_YAS9oglv_BEnd6jpk2Y794g1BlYRbSn-kvfcVt4A0_O3CyrrY1q3P8Iv9eUfdo1-F1us7GFLnxK0dJ7KBEcG0=w2400</t>
+  </si>
+  <si>
+    <t>We got engaged!</t>
+  </si>
+  <si>
+    <t>I proposed to Gia using a cool looking comic book puzzle. Sponsored by Etsy!</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/nBUI-zoN7YHfQ18OfLox1rbUJJQCjIqKaaxG32zjtORBuNjo6_Xi1orBJwHSSlvt4W23ZqAZN-sEe9yk1vTnXYXdLDIZcto9ublyNYWSvn4T6BIDVrdccoZlTGTH2aZ1aomHXaQcVrQ=w2400</t>
   </si>
   <si>
     <t>Get shared photo link</t>
@@ -1033,7 +1042,18 @@
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="B31" s="4"/>
+      <c r="A31" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="6">
+        <v>44196.0</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="B32" s="4"/>
@@ -3953,11 +3973,12 @@
     <hyperlink r:id="rId2" ref="D28"/>
     <hyperlink r:id="rId3" ref="D29"/>
     <hyperlink r:id="rId4" ref="D30"/>
+    <hyperlink r:id="rId5" ref="D31"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -3977,22 +3998,22 @@
     <row r="1" ht="15.75" customHeight="1"/>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1"/>

</xml_diff>